<commit_message>
Updte ReadPropertiesFromExcel test to not include dynamic properties - therefore tests will stay static.
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/ReadPropertiesFromExcel/Data/CO-SWSI-Control.xlsx
+++ b/test/regression/commands/general/ReadPropertiesFromExcel/Data/CO-SWSI-Control.xlsx
@@ -16,43 +16,42 @@
     <sheet name="Config_FP" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="BooleanProperty">Config!$E$39</definedName>
-    <definedName name="CurrentMonth" comment="Current month (as month number 1-12)">Config!$E$8</definedName>
-    <definedName name="CurrentMonthDate" comment="Current month (as date) for which SWSI is being computed">Config!$E$7</definedName>
-    <definedName name="CurrentMonthDateText">Config!$F$7</definedName>
-    <definedName name="CurrentWaterYearEndDate" comment="End of the current water year.">Config!$E$22</definedName>
-    <definedName name="CurrentWaterYearStartDate" comment="Start of the current water year.">Config!$E$21</definedName>
-    <definedName name="DoubleProperty">Config!$E$38</definedName>
-    <definedName name="HistoricalPeriodEndDate" comment="End of the normal period for calculating ranked SWSI statistics, global for all locations.">Config!$E$24</definedName>
-    <definedName name="HistoricalPeriodStartDate" comment="Start of the normal period for calculating ranked SWSI statistics, global for all locations.">Config!$E$23</definedName>
-    <definedName name="InputPeriodEndDate" comment="End of the input period when reading historical data, go to end of current water year.">Config!$E$29</definedName>
-    <definedName name="InputPeriodStartDate" comment="Start of the input period when reading historical data, extra month is needed for forward shift fror some data.">Config!$E$28</definedName>
-    <definedName name="IntegerProperty">Config!$E$50</definedName>
-    <definedName name="LastHistoricalForecastDate" comment="Date for last historical forecast date (after this all forecasts are truly forecasts), December of previous calendar year.">Config!$E$30</definedName>
-    <definedName name="MaxHUCForecastGageCount" comment="Maximum number of HUC forecast gage stations, used to size some output reports.">Config!$E$36</definedName>
-    <definedName name="MaxHUCReservoirCount" comment="Maximum number of HUC reservoirs, used to size some output reports.">Config!$E$35</definedName>
-    <definedName name="MaxHUCStreamGageCount" comment="Maximum number of HUC stream gages, used to size some output reports.">Config!$E$34</definedName>
-    <definedName name="NaturalFlowOverrideDate" comment="Date for which natural flow data are being provided, to fill values in available data.">#REF!</definedName>
-    <definedName name="NextMonthDate" comment="Next month (as date)">Config!$E$10</definedName>
-    <definedName name="NRCSForecastPublicationDate" comment="Used to look up the NRCS forecasts from web service request.">Config!$E$11</definedName>
-    <definedName name="NRCSForecastPublicationDateText">Config!$F$11</definedName>
-    <definedName name="NullProperty">Config!$E$49</definedName>
-    <definedName name="NumberAsBooleanFalseProperty">Config!$E$41</definedName>
-    <definedName name="NumberAsBooleanTrueProperty">Config!$E$40</definedName>
-    <definedName name="PreviousMonthDate" comment="Previous month (as date)">Config!$E$9</definedName>
-    <definedName name="RecentPeriodGraphEndDate" comment="End of the recent period for graphs of the last few years.">Config!$E$32</definedName>
-    <definedName name="RecentPeriodGraphStartDate" comment="Start of the recent period for graphs of the last few years.">Config!$E$31</definedName>
-    <definedName name="RecentPeriodStartDate" comment="Start of the recent period (years after historical period).">Config!$E$25</definedName>
-    <definedName name="SWSIForecastPeriodByMonth" comment="Forecast volume period to use by month.">Config_FP!$A$2:$C$7</definedName>
-    <definedName name="SWSIForecastPeriodByMonthDefault" comment="Forecast period to use for each month of the SWSI analysis, default values.">Config_FP!$B$2:$B$7</definedName>
-    <definedName name="SWSIForecastPeriodByMonthRioGrande" comment="Forecast period to use for each month of the SWSI analysis, Rio Grande basin values.">Config_FP!$C$2:$C$7</definedName>
-    <definedName name="Text0AsBooleanFalseProperty">Config!$E$47</definedName>
-    <definedName name="Text1AsBooleanTrueProperty">Config!$E$46</definedName>
-    <definedName name="TextAsDateTimeProperty">Config!$E$48</definedName>
-    <definedName name="TextFalseAsBooleanFalseProperty">Config!$E$45</definedName>
-    <definedName name="TextNoAsBooleanFalseProperty">Config!$E$43</definedName>
-    <definedName name="TextTrueAsBooleanTrueProperty">Config!$E$44</definedName>
-    <definedName name="TextYesAsBooleanTrueProperty">Config!$E$42</definedName>
+    <definedName name="ExcelTestBooleanProperty">Config!$E$39</definedName>
+    <definedName name="ExcelTestCurrentMonth" comment="Current month (as month number 1-12)">Config!$E$8</definedName>
+    <definedName name="ExcelTestCurrentMonthDate" comment="Current month (as date) for which SWSI is being computed">Config!$E$7</definedName>
+    <definedName name="ExcelTestCurrentMonthDateText">Config!$F$7</definedName>
+    <definedName name="ExcelTestCurrentWaterYearEndDate" comment="End of the current water year.">Config!$E$22</definedName>
+    <definedName name="ExcelTestCurrentWaterYearStartDate" comment="Start of the current water year.">Config!$E$21</definedName>
+    <definedName name="ExcelTestDoubleProperty">Config!$E$38</definedName>
+    <definedName name="ExcelTestHistoricalPeriodEndDate" comment="End of the normal period for calculating ranked SWSI statistics, global for all locations.">Config!$E$24</definedName>
+    <definedName name="ExcelTestHistoricalPeriodStartDate" comment="Start of the normal period for calculating ranked SWSI statistics, global for all locations.">Config!$E$23</definedName>
+    <definedName name="ExcelTestInputPeriodEndDate" comment="End of the input period when reading historical data, go to end of current water year.">Config!$E$29</definedName>
+    <definedName name="ExcelTestInputPeriodStartDate" comment="Start of the input period when reading historical data, extra month is needed for forward shift fror some data.">Config!$E$28</definedName>
+    <definedName name="ExcelTestIntegerProperty">Config!$E$50</definedName>
+    <definedName name="ExcelTestLastHistoricalForecastDate" comment="Date for last historical forecast date (after this all forecasts are truly forecasts), December of previous calendar year.">Config!$E$30</definedName>
+    <definedName name="ExcelTestMaxHUCForecastGageCount" comment="Maximum number of HUC forecast gage stations, used to size some output reports.">Config!$E$36</definedName>
+    <definedName name="ExcelTestMaxHUCReservoirCount" comment="Maximum number of HUC reservoirs, used to size some output reports.">Config!$E$35</definedName>
+    <definedName name="ExcelTestMaxHUCStreamGageCount" comment="Maximum number of HUC stream gages, used to size some output reports.">Config!$E$34</definedName>
+    <definedName name="ExcelTestNextMonthDate" comment="Next month (as date)">Config!$E$10</definedName>
+    <definedName name="ExcelTestNRCSForecastPublicationDate" comment="Used to look up the NRCS forecasts from web service request.">Config!$E$11</definedName>
+    <definedName name="ExcelTestNRCSForecastPublicationDateText">Config!$F$11</definedName>
+    <definedName name="ExcelTestNullProperty">Config!$E$49</definedName>
+    <definedName name="ExcelTestNumberAsBooleanFalseProperty">Config!$E$41</definedName>
+    <definedName name="ExcelTestNumberAsBooleanTrueProperty">Config!$E$40</definedName>
+    <definedName name="ExcelTestPreviousMonthDate" comment="Previous month (as date)">Config!$E$9</definedName>
+    <definedName name="ExcelTestRecentPeriodGraphEndDate" comment="End of the recent period for graphs of the last few years.">Config!$E$32</definedName>
+    <definedName name="ExcelTestRecentPeriodGraphStartDate" comment="Start of the recent period for graphs of the last few years.">Config!$E$31</definedName>
+    <definedName name="ExcelTestRecentPeriodStartDate" comment="Start of the recent period (years after historical period).">Config!$E$25</definedName>
+    <definedName name="ExcelTestSWSIForecastPeriodByMonth" comment="Forecast volume period to use by month.">Config_FP!$A$2:$C$7</definedName>
+    <definedName name="ExcelTestSWSIForecastPeriodByMonthDefault" comment="Forecast period to use for each month of the SWSI analysis, default values.">Config_FP!$B$2:$B$7</definedName>
+    <definedName name="ExcelTestSWSIForecastPeriodByMonthRioGrande" comment="Forecast period to use for each month of the SWSI analysis, Rio Grande basin values.">Config_FP!$C$2:$C$7</definedName>
+    <definedName name="ExcelTestText0AsBooleanFalseProperty">Config!$E$47</definedName>
+    <definedName name="ExcelTestText1AsBooleanTrueProperty">Config!$E$46</definedName>
+    <definedName name="ExcelTestTextAsDateTimeProperty">Config!$E$48</definedName>
+    <definedName name="ExcelTestTextFalseAsBooleanFalseProperty">Config!$E$45</definedName>
+    <definedName name="ExcelTestTextNoAsBooleanFalseProperty">Config!$E$43</definedName>
+    <definedName name="ExcelTestTextTrueAsBooleanTrueProperty">Config!$E$44</definedName>
+    <definedName name="ExcelTestTextYesAsBooleanTrueProperty">Config!$E$42</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -878,7 +877,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +933,7 @@
         <v>42125</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f>TEXT(CurrentMonthDate,"yyyy-mm")</f>
+        <f>TEXT(ExcelTestCurrentMonthDate,"yyyy-mm")</f>
         <v>2015-05</v>
       </c>
       <c r="G7" t="s">
@@ -949,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="6">
-        <f>MONTH(CurrentMonthDate)</f>
+        <f>MONTH(ExcelTestCurrentMonthDate)</f>
         <v>5</v>
       </c>
       <c r="F8" s="6"/>
@@ -965,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="4">
-        <f>IF(MONTH(CurrentMonthDate)=1,DATE((YEAR(CurrentMonthDate)-1),12,1),DATE(YEAR(CurrentMonthDate),(MONTH(CurrentMonthDate)-1),1))</f>
+        <f>IF(MONTH(ExcelTestCurrentMonthDate)=1,DATE((YEAR(ExcelTestCurrentMonthDate)-1),12,1),DATE(YEAR(ExcelTestCurrentMonthDate),(MONTH(ExcelTestCurrentMonthDate)-1),1))</f>
         <v>42095</v>
       </c>
       <c r="F9" s="4"/>
@@ -981,7 +980,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="4">
-        <f>DATE(YEAR(CurrentMonthDate),(MONTH(CurrentMonthDate)+1),1)</f>
+        <f>DATE(YEAR(ExcelTestCurrentMonthDate),(MONTH(ExcelTestCurrentMonthDate)+1),1)</f>
         <v>42156</v>
       </c>
       <c r="F10" s="4"/>
@@ -997,11 +996,11 @@
         <v>5</v>
       </c>
       <c r="E11" s="15">
-        <f>CurrentMonthDate</f>
+        <f>ExcelTestCurrentMonthDate</f>
         <v>42125</v>
       </c>
       <c r="F11" s="15" t="str">
-        <f>TEXT(NRCSForecastPublicationDate,"YYYY-MM-DD hh:mm:ss")</f>
+        <f>TEXT(ExcelTestNRCSForecastPublicationDate,"YYYY-MM-DD hh:mm:ss")</f>
         <v>2015-05-01 00:00:00</v>
       </c>
       <c r="G11" t="s">
@@ -1016,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F12" s="8"/>
@@ -1032,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F13" s="8"/>
@@ -1048,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F14" s="8"/>
@@ -1064,7 +1063,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F15" s="8"/>
@@ -1080,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,3,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,3,FALSE)</f>
         <v>MAY-SEP</v>
       </c>
       <c r="F16" s="8"/>
@@ -1096,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F17" s="8"/>
@@ -1112,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F18" s="8"/>
@@ -1128,7 +1127,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="8" t="str">
-        <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
+        <f>VLOOKUP(ExcelTestCurrentMonth,ExcelTestSWSIForecastPeriodByMonth,2,FALSE)</f>
         <v>MAY-JUL</v>
       </c>
       <c r="F19" s="8"/>
@@ -1167,7 +1166,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="4">
-        <f>DATE((YEAR(CurrentWaterYearStartDate)+1),9,30)</f>
+        <f>DATE((YEAR(ExcelTestCurrentWaterYearStartDate)+1),9,30)</f>
         <v>42277</v>
       </c>
       <c r="F22" s="4"/>
@@ -1213,7 +1212,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="4">
-        <f>DATE(YEAR(HistoricalPeriodEndDate),(MONTH(HistoricalPeriodEndDate)+1),1)</f>
+        <f>DATE(YEAR(ExcelTestHistoricalPeriodEndDate),(MONTH(ExcelTestHistoricalPeriodEndDate)+1),1)</f>
         <v>40452</v>
       </c>
       <c r="F25" s="4"/>
@@ -1229,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="4">
-        <f>CurrentWaterYearEndDate</f>
+        <f>ExcelTestCurrentWaterYearEndDate</f>
         <v>42277</v>
       </c>
       <c r="F26" s="4"/>
@@ -1249,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="4">
-        <f>DATE(YEAR(HistoricalPeriodStartDate),(MONTH(HistoricalPeriodStartDate)-1),1)</f>
+        <f>DATE(YEAR(ExcelTestHistoricalPeriodStartDate),(MONTH(ExcelTestHistoricalPeriodStartDate)-1),1)</f>
         <v>25812</v>
       </c>
       <c r="F28" s="4"/>
@@ -1265,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="4">
-        <f>CurrentWaterYearEndDate</f>
+        <f>ExcelTestCurrentWaterYearEndDate</f>
         <v>42277</v>
       </c>
       <c r="F29" s="4"/>
@@ -1281,7 +1280,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="4">
-        <f>DATE(YEAR(CurrentWaterYearStartDate),12,1)</f>
+        <f>DATE(YEAR(ExcelTestCurrentWaterYearStartDate),12,1)</f>
         <v>41974</v>
       </c>
       <c r="F30" s="4"/>
@@ -1312,7 +1311,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="4">
-        <f>CurrentWaterYearEndDate</f>
+        <f>ExcelTestCurrentWaterYearEndDate</f>
         <v>42277</v>
       </c>
       <c r="F32" s="4"/>

</xml_diff>